<commit_message>
trips adding in backend from frontend done
</commit_message>
<xml_diff>
--- a/resources/assigntrip.xlsx
+++ b/resources/assigntrip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Techidol solutions\CRM\crm_dashboard\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE2ED13-573A-45CE-BD2A-3EBBBB8C34C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8611C4-30DE-4AA2-A269-DAD3581BA9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>MP04CT1234</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>Start Km</t>
-  </si>
-  <si>
-    <t>End Km</t>
   </si>
   <si>
     <t>Kolar</t>
@@ -499,7 +496,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -533,31 +530,25 @@
       <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>2024</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1">
         <v>45393</v>
       </c>
       <c r="F2">
         <v>55636</v>
-      </c>
-      <c r="G2">
-        <v>75143</v>
       </c>
       <c r="K2" s="1"/>
     </row>
@@ -566,22 +557,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>2024</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="1">
         <v>45394</v>
       </c>
       <c r="F3">
         <v>87442</v>
-      </c>
-      <c r="G3">
-        <v>99273</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -590,22 +578,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <v>2024</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="1">
         <v>45395</v>
       </c>
       <c r="F4">
         <v>26352</v>
-      </c>
-      <c r="G4">
-        <v>87352</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -614,22 +599,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5">
         <v>2024</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="1">
         <v>45396</v>
       </c>
       <c r="F5">
         <v>10937</v>
-      </c>
-      <c r="G5">
-        <v>15735</v>
       </c>
       <c r="K5" s="1"/>
     </row>
@@ -638,22 +620,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>2024</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="1">
         <v>45397</v>
       </c>
       <c r="F6">
         <v>87245</v>
-      </c>
-      <c r="G6">
-        <v>99783</v>
       </c>
       <c r="K6" s="1"/>
     </row>
@@ -662,22 +641,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7">
         <v>2024</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="1">
         <v>45398</v>
       </c>
       <c r="F7">
         <v>67536</v>
-      </c>
-      <c r="G7">
-        <v>98917</v>
       </c>
       <c r="K7" s="1"/>
     </row>
@@ -686,22 +662,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8">
         <v>2024</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="1">
         <v>45399</v>
       </c>
       <c r="F8">
         <v>96314</v>
-      </c>
-      <c r="G8">
-        <v>152939</v>
       </c>
       <c r="K8" s="1"/>
     </row>
@@ -710,22 +683,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9">
         <v>2024</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="1">
         <v>45400</v>
       </c>
       <c r="F9">
         <v>38263</v>
-      </c>
-      <c r="G9">
-        <v>76356</v>
       </c>
       <c r="K9" s="1"/>
     </row>
@@ -734,22 +704,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10">
         <v>2024</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" s="1">
         <v>45401</v>
       </c>
       <c r="F10">
         <v>76545</v>
-      </c>
-      <c r="G10">
-        <v>133567</v>
       </c>
       <c r="K10" s="1"/>
     </row>
@@ -758,22 +725,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11">
         <v>2024</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" s="1">
         <v>45402</v>
       </c>
       <c r="F11">
         <v>72634</v>
-      </c>
-      <c r="G11">
-        <v>322133</v>
       </c>
       <c r="K11" s="1"/>
     </row>
@@ -782,22 +746,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12">
         <v>2024</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="1">
         <v>45403</v>
       </c>
       <c r="F12">
         <v>16253</v>
-      </c>
-      <c r="G12">
-        <v>76253</v>
       </c>
       <c r="K12" s="1"/>
     </row>
@@ -806,22 +767,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13">
         <v>2024</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E13" s="1">
         <v>45404</v>
       </c>
       <c r="F13">
         <v>42262</v>
-      </c>
-      <c r="G13">
-        <v>87635</v>
       </c>
       <c r="K13" s="1"/>
     </row>
@@ -830,22 +788,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14">
         <v>2024</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="1">
         <v>45405</v>
       </c>
       <c r="F14">
         <v>76543</v>
-      </c>
-      <c r="G14">
-        <v>271533</v>
       </c>
       <c r="K14" s="1"/>
     </row>
@@ -854,22 +809,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>2024</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" s="1">
         <v>45406</v>
       </c>
       <c r="F15">
         <v>92727</v>
-      </c>
-      <c r="G15">
-        <v>263234</v>
       </c>
       <c r="K15" s="1"/>
     </row>
@@ -878,22 +830,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16">
         <v>2024</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16" s="1">
         <v>45407</v>
       </c>
       <c r="F16">
         <v>27364</v>
-      </c>
-      <c r="G16">
-        <v>122372</v>
       </c>
       <c r="K16" s="1"/>
     </row>

</xml_diff>

<commit_message>
assign trip excel data changes
</commit_message>
<xml_diff>
--- a/resources/assigntrip.xlsx
+++ b/resources/assigntrip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Techidol solutions\CRM\crm_dashboard\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9638779-9655-41BC-9B28-E719272FE87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D877ADC-1AC8-44C4-94EE-34C8B4D7307E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>MP04CT1234</t>
   </si>
   <si>
-    <t>MP04CT1235</t>
-  </si>
-  <si>
     <t>MP04CT1236</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
     <t>Vehicle Registration Number</t>
   </si>
   <si>
-    <t>MP04CT1244</t>
-  </si>
-  <si>
     <t>MP04CT1247</t>
   </si>
   <si>
@@ -148,6 +142,12 @@
   </si>
   <si>
     <t>BSK-06</t>
+  </si>
+  <si>
+    <t>MP04CT1237</t>
+  </si>
+  <si>
+    <t>MP04CT1239</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -504,22 +504,22 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -527,13 +527,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>2024</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E2" s="1">
         <v>45393</v>
@@ -548,13 +548,13 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>2024</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1">
         <v>45394</v>
@@ -569,13 +569,13 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4">
         <v>2024</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1">
         <v>45387</v>
@@ -587,16 +587,16 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>2024</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1">
         <v>45396</v>
@@ -608,16 +608,16 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>2024</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1">
         <v>45397</v>
@@ -629,16 +629,16 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>2024</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E7" s="1">
         <v>45398</v>
@@ -650,16 +650,16 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>2024</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E8" s="1">
         <v>45399</v>
@@ -671,16 +671,16 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>2024</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E9" s="1">
         <v>45400</v>
@@ -692,16 +692,16 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>2024</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" s="1">
         <v>45401</v>
@@ -713,16 +713,16 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11">
         <v>2024</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E11" s="1">
         <v>45402</v>
@@ -734,16 +734,16 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>2024</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E12" s="1">
         <v>45403</v>
@@ -755,16 +755,16 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>2024</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E13" s="1">
         <v>45404</v>
@@ -776,16 +776,16 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <v>2024</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E14" s="1">
         <v>45405</v>
@@ -797,16 +797,16 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>2024</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E15" s="1">
         <v>45406</v>
@@ -818,16 +818,16 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16">
         <v>2024</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E16" s="1">
         <v>45407</v>

</xml_diff>